<commit_message>
Introduction done + Thesis structure updated
</commit_message>
<xml_diff>
--- a/Thesis-Structure.xlsx
+++ b/Thesis-Structure.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noiseux1523/Dropbox/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noiseux1523/Dropbox/Memoire/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14900" windowHeight="16640" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="27200" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>DEDICATION</t>
   </si>
@@ -177,6 +177,15 @@
   </si>
   <si>
     <t>APPENDICES</t>
+  </si>
+  <si>
+    <t>Internal Validity</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>TOTAL CONTENT</t>
   </si>
 </sst>
 </file>
@@ -497,300 +506,485 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A57"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="88.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="B39">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="B42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="B43">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="B45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="B46">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+      <c r="B47">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="B48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+      <c r="B50">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+      <c r="B51">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+      <c r="B52">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+      <c r="B54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+      <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+      <c r="B56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>49</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B59">
+        <f>SUM(B1:B58)</f>
+        <v>81.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B60">
+        <f>SUM(B1:B4,B10:B56)</f>
+        <v>74.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>